<commit_message>
docs: update dataset documentation
</commit_message>
<xml_diff>
--- a/datasets/mlsum_fr_train_subset_v1.0.0.schild.xlsx
+++ b/datasets/mlsum_fr_train_subset_v1.0.0.schild.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHILDEW\Documents\INTERACTIVE-CLUSTERING\github-interactive-clustering-comparative-study\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCHILDEW\Documents\INTERACTIVE-CLUSTERING\interactive-clustering-comparative-study\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7100" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7105" uniqueCount="1122">
   <si>
     <t>title</t>
   </si>
@@ -3412,12 +3412,6 @@
     <t>faits-divers</t>
   </si>
   <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>DOI</t>
-  </si>
-  <si>
     <t>VERSION</t>
   </si>
   <si>
@@ -3428,9 +3422,6 @@
   </si>
   <si>
     <t>LICENSE - ACCESS RIGHT</t>
-  </si>
-  <si>
-    <t>TITLE</t>
   </si>
   <si>
     <t>MLSUM: The Multilingual Summarization Corpus</t>
@@ -3473,9 +3464,6 @@
     <t>Thomas SCIALOM, Paul-Alexis DRAY, Sylvain LAMPRIER, Benjamin PIWOWARSKI, Jacopo STAIANO</t>
   </si>
   <si>
-    <t>AUTHORS (creation)</t>
-  </si>
-  <si>
     <t>AUTHORS (edition)</t>
   </si>
   <si>
@@ -3483,9 +3471,6 @@
   </si>
   <si>
     <t>DESCRIPTION (edition)</t>
-  </si>
-  <si>
-    <t>DESCRIPTION (abstract)</t>
   </si>
   <si>
     <r>
@@ -3506,19 +3491,19 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>For constraints annotation experiment based on data similarity, this dataset have been subsetted (</t>
-    </r>
+    <t>Subset of 'MLSUM: The Multilingual Summarization Corpus' for constraints annotation experiment</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <i/>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>randomly pick 75 articles in the following 14 most used topics: 'economie', 'politique', 'sport', 'planete' (renamed in 'ecologie'), 'sciences', 'police-justice', 'disparitions', 'emploi', 'sante', 'musiques', 'arts', 'educations', 'climat' (renamed in 'meteo'), 'immobilier'</t>
+      <t>[EN] Subset of 'MLSUM: The Multilingual Summarization Corpus' for constraints annotation experiment.</t>
     </r>
     <r>
       <rPr>
@@ -3528,18 +3513,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) and filtered (</t>
+      <t xml:space="preserve">
+</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>keep articles that have an obvious topics regarding their titles, without their bodies</t>
+      <t>Description</t>
     </r>
     <r>
       <rPr>
@@ -3549,18 +3535,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>). Two reviewers have working on this task in order to limit the subjectivity of the filtering. This subsetted dataset is used (1) to estimate needed time to annotate titles similarity with constraints (</t>
+      <t xml:space="preserve">: MLSUM is a dataset of newspappers articles aimed at training summaring model. We use it for a constraints annotation experiment on newspapper titles according to their topic classification.
+</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>MUST-LINK, CANNOT-LINK</t>
+      <t>Content</t>
     </r>
     <r>
       <rPr>
@@ -3570,18 +3557,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>) and (2) to test interactive clustering methodology (</t>
+      <t xml:space="preserve">: For constraints annotation experiment based on data similarity, this dataset have been subsetted (randomly pick 75 articles in the following 14 most used topics: 'economie', 'politique', 'sport', 'planete' (renamed in 'ecologie'), 'sciences', 'police-justice', 'disparitions', 'emploi', 'sante', 'musiques', 'arts', 'educations', 'climat' (renamed in 'meteo'), 'immobilier') and filtered (keep articles that have an obvious topics regarding their titles, without their bodies). Two reviewers have working on this task in order to limit the subjectivity of the filtering. This subsetted dataset is used (1) to estimate needed time to annotate titles similarity with constraints (MUST-LINK, CANNOT-LINK) and (2) to test interactive clustering methodology (constraints annotation and constrained clustering).
+Origin: The dataset is bassed on the original 'MLSUM: The Multilingual Summarization Corpus' dataset (https://doi.org/10.48550/arXiv.2004.14900).
+</t>
     </r>
     <r>
       <rPr>
-        <i/>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>constraints annotation and constrained clustering</t>
+      <t>----
+[FR] Echantillon de 'MLSUM: The Multilingual Summarization Corpus' pour une expériemnt d'annotation de contraintes.</t>
     </r>
     <r>
       <rPr>
@@ -3591,15 +3581,109 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>).</t>
+      <t xml:space="preserve">
+</t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : MLSUM est un ensemble de données d'articles de journaux destinés à l'entraînement d'un modèle de résumé automatique. Nous l'utilisons pour une expérience d'annotation de contraintes sur des titres de journaux en fonction de leur classification thématique.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contenu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Pour une expérience d'annotation de contraintes basée sur la similarité des données, cet ensemble de données a été échantillonné (sélectionner au hasard de 75 articles dans les 14 sujets les plus utilisés : 'économie', 'politique', 'sport', 'planète' (renommé en « écologie »). ), 'sciences', 'police-justice', 'disparitions', 'emploi', 'sante', 'musiques', 'arts', 'éducations', 'climat' (renommé en 'meteo'), 'immobilier' ) et filtré (conserver les articles qui ont un sujet évident par rapport à leur titre, sans leur corps). Deux relecteurs ont travaillé sur cette tâche afin de limiter la subjectivité du filtrage. Ce sous-ensemble de données est utilisé (1) pour estimer le temps nécessaire pour annoter la similarité des titres avec des contraintes (MUST-LINK, CANNOT-LINK) et (2) pour tester la méthodologie de clustering interactif (annotation de contraintes et clustering contraint).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Origine</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : L'ensemble de données est basé sur l'ensemble de données original 'MLSUM : The Multilingual Summarization Corpus' (https://doi.org/10.48550/arXiv.2004.14900).
+</t>
+    </r>
+  </si>
+  <si>
+    <t>DOI (original)</t>
+  </si>
+  <si>
+    <t>DOI (edition)</t>
+  </si>
+  <si>
+    <t>10.5281/zenodo.8399302</t>
+  </si>
+  <si>
+    <t>TITLE (original)</t>
+  </si>
+  <si>
+    <t>TITLE (edition)</t>
+  </si>
+  <si>
+    <t>AUTHORS (original)</t>
+  </si>
+  <si>
+    <t>DESCRIPTION (original)</t>
+  </si>
+  <si>
+    <t>DATE (original)</t>
+  </si>
+  <si>
+    <t>DATE (edition)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3665,14 +3749,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3722,7 +3798,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3756,6 +3832,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -10372,104 +10451,132 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="255.7109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>1097</v>
+        <v>1116</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>1110</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>1114</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B4" s="10">
+        <v>43981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>1113</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>1116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B6" s="10">
-        <v>43981</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>1092</v>
+      <c r="B5" s="11" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>1117</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>1101</v>
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="8" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B10" s="14">
+        <v>45201</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>1102</v>
+        <v>1114</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>1099</v>
       </c>
     </row>
   </sheetData>
@@ -10483,8 +10590,8 @@
   <dimension ref="A1:G1051"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10505,19 +10612,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>